<commit_message>
paro 2018 correción formato
</commit_message>
<xml_diff>
--- a/webscrapping final/Bases finales/base_2018.xlsx
+++ b/webscrapping final/Bases finales/base_2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\SED---Cuantitativo\webscrapping final\Bases finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D1C9C84-3799-4333-A50E-402B22D1C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671FEC92-31D3-4374-85C5-1C62100A7158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_PAROS_UNIFICADOS_2019 (5)" sheetId="2" r:id="rId1"/>
@@ -24,8 +24,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" keepAlive="1" name="Consulta - BASE_PAROS_UNIFICADOS_2019 (4)" description="Conexión a la consulta 'BASE_PAROS_UNIFICADOS_2019 (4)' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - BASE_PAROS_UNIFICADOS_2019 (4)" description="Conexión a la consulta 'BASE_PAROS_UNIFICADOS_2019 (4)' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;BASE_PAROS_UNIFICADOS_2019 (4)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [BASE_PAROS_UNIFICADOS_2019 (4)]"/>
   </connection>
 </connections>
@@ -395,8 +395,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -531,6 +531,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -829,7 +837,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -872,13 +880,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -910,6 +919,7 @@
     <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
     <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,7 +992,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatosExternos_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="17">
     <queryTableFields count="16">
       <queryTableField id="1" name="fecha_inicio" tableColumnId="1"/>
@@ -1007,25 +1017,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="BASE_PAROS_UNIFICADOS_2019__4" displayName="BASE_PAROS_UNIFICADOS_2019__4" ref="A1:P7" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:P7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="BASE_PAROS_UNIFICADOS_2019__4" displayName="BASE_PAROS_UNIFICADOS_2019__4" ref="A1:P7" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:P7" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="16">
-    <tableColumn id="1" uniqueName="1" name="fecha_inicio" queryTableFieldId="1" dataDxfId="14"/>
-    <tableColumn id="2" uniqueName="2" name="fecha_fin" queryTableFieldId="2" dataDxfId="13"/>
-    <tableColumn id="3" uniqueName="3" name="ciudad" queryTableFieldId="3" dataDxfId="12"/>
-    <tableColumn id="4" uniqueName="4" name="organizaciones_sindicales" queryTableFieldId="4" dataDxfId="11"/>
-    <tableColumn id="5" uniqueName="5" name="tipo_movilizacion" queryTableFieldId="5" dataDxfId="10"/>
-    <tableColumn id="6" uniqueName="6" name="duracion_dias" queryTableFieldId="6"/>
-    <tableColumn id="7" uniqueName="7" name="razones_paro" queryTableFieldId="7" dataDxfId="9"/>
-    <tableColumn id="8" uniqueName="8" name="resumen" queryTableFieldId="8" dataDxfId="8"/>
-    <tableColumn id="9" uniqueName="9" name="fuentes_presentes" queryTableFieldId="9" dataDxfId="7"/>
-    <tableColumn id="10" uniqueName="10" name="url_1" queryTableFieldId="10" dataDxfId="6"/>
-    <tableColumn id="11" uniqueName="11" name="url_2" queryTableFieldId="11" dataDxfId="5"/>
-    <tableColumn id="12" uniqueName="12" name="url_3" queryTableFieldId="12" dataDxfId="4"/>
-    <tableColumn id="13" uniqueName="13" name="url_4" queryTableFieldId="13" dataDxfId="3"/>
-    <tableColumn id="14" uniqueName="14" name="url_5" queryTableFieldId="14" dataDxfId="2"/>
-    <tableColumn id="15" uniqueName="15" name="url_6" queryTableFieldId="15" dataDxfId="1"/>
-    <tableColumn id="16" uniqueName="16" name="url_7" queryTableFieldId="16" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="fecha_inicio" queryTableFieldId="1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="fecha_fin" queryTableFieldId="2" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="ciudad" queryTableFieldId="3" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="organizaciones_sindicales" queryTableFieldId="4" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="tipo_movilizacion" queryTableFieldId="5" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="6" name="duracion_dias" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="7" name="razones_paro" queryTableFieldId="7" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="8" name="resumen" queryTableFieldId="8" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="9" name="fuentes_presentes" queryTableFieldId="9" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="10" name="url_1" queryTableFieldId="10" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" uniqueName="11" name="url_2" queryTableFieldId="11" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" uniqueName="12" name="url_3" queryTableFieldId="12" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" uniqueName="13" name="url_4" queryTableFieldId="13" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" uniqueName="14" name="url_5" queryTableFieldId="14" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" uniqueName="15" name="url_6" queryTableFieldId="15" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" uniqueName="16" name="url_7" queryTableFieldId="16" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1327,10 +1337,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1402,43 +1414,46 @@
       <c r="B2" s="1">
         <v>43152</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>81</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="2" t="s">
+      <c r="K2" t="s">
+        <v>76</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1449,46 +1464,46 @@
       <c r="B3" s="1">
         <v>43229</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>78</v>
       </c>
       <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>84</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>85</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>86</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="L3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M3" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P3" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1499,28 +1514,28 @@
       <c r="B4" s="1">
         <v>43307</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>89</v>
       </c>
       <c r="F4">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>93</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -1529,16 +1544,16 @@
       <c r="L4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" t="s">
         <v>96</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" t="s">
         <v>97</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P4" s="2" t="s">
+      <c r="O4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P4" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1549,46 +1564,46 @@
       <c r="B5" s="1">
         <v>43386</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
         <v>98</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" t="s">
         <v>99</v>
       </c>
       <c r="F5">
-        <v>330</v>
-      </c>
-      <c r="G5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>101</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" t="s">
         <v>102</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>103</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" t="s">
         <v>104</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" t="s">
         <v>105</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" t="s">
         <v>106</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P5" s="2" t="s">
+      <c r="N5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1599,46 +1614,46 @@
       <c r="B6" s="1">
         <v>43397</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>89</v>
       </c>
       <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
         <v>108</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" t="s">
         <v>92</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" t="s">
         <v>111</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" t="s">
         <v>113</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" t="s">
         <v>114</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" t="s">
         <v>115</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1649,59 +1664,65 @@
       <c r="B7" s="1">
         <v>43432</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="2" t="s">
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" t="s">
         <v>117</v>
       </c>
       <c r="F7">
-        <v>10</v>
-      </c>
-      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
         <v>118</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>118</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>81</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="P7" s="2" t="s">
+      <c r="J7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O7" t="s">
+        <v>76</v>
+      </c>
+      <c r="P7" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{49B0F36A-D6B5-4262-81B1-818BD1068C0E}"/>
+    <hyperlink ref="K4" r:id="rId2" xr:uid="{3BEB4F51-DB85-41AB-9353-F225624F69C1}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{8A1E86D4-1E92-4DD4-87CF-12562C07BC38}"/>
+    <hyperlink ref="J2" r:id="rId4" xr:uid="{A55013BD-3749-43BA-A5CA-172B96248001}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>